<commit_message>
Battery percentage order reversed
</commit_message>
<xml_diff>
--- a/Battery information.xlsx
+++ b/Battery information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\S-car-lett-A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AF03D-A707-4B4F-A19D-0AC1B3B664ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1D9D81-FB27-497E-BAB7-EF9D5330C0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E4B752A-BD50-4D06-9001-C393B2186BBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E4B752A-BD50-4D06-9001-C393B2186BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="General information" sheetId="1" r:id="rId1"/>
@@ -135,8 +135,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -177,15 +177,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,22 +192,10 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="172" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="165" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -218,6 +205,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -236,8 +235,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02199FD1-2069-47B5-BC17-F004A01CC3EB}" name="Main" displayName="Main" ref="A1:B10" totalsRowShown="0">
   <autoFilter ref="A1:B10" xr:uid="{02199FD1-2069-47B5-BC17-F004A01CC3EB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0C2E4F09-43D9-4DC2-9693-333458FF0A2B}" name="PROPERTY" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4DC600EE-AFDE-4F3E-93A9-61612CD59CC6}" name="VALUE" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0C2E4F09-43D9-4DC2-9693-333458FF0A2B}" name="PROPERTY" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4DC600EE-AFDE-4F3E-93A9-61612CD59CC6}" name="VALUE" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -246,9 +245,12 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8A80B4EE-F6A2-49B6-A147-24F5560B73F5}" name="Mapping" displayName="Mapping" ref="A1:B102" totalsRowShown="0">
   <autoFilter ref="A1:B102" xr:uid="{8A80B4EE-F6A2-49B6-A147-24F5560B73F5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B102">
+    <sortCondition descending="1" ref="A1:A102"/>
+  </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{499E6699-319F-41F6-82A4-A74BBC1E034A}" name="VOLTAGE" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{158FA4FB-5773-4312-87ED-4A25463C8064}" name="PERCENTAGE" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{499E6699-319F-41F6-82A4-A74BBC1E034A}" name="VOLTAGE" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{158FA4FB-5773-4312-87ED-4A25463C8064}" name="PERCENTAGE" dataDxfId="5" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -258,11 +260,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B280702-4076-4718-BB89-8416DF14CC68}" name="Events" displayName="Events" ref="A1:E6" totalsRowShown="0">
   <autoFilter ref="A1:E6" xr:uid="{8B280702-4076-4718-BB89-8416DF14CC68}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28BC94F7-F562-4A52-A433-A77216BAF33C}" name="DATE" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{2F3C2F88-E388-48C8-B6EB-07F35CF45C6F}" name="NAME" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{1357C874-AE04-46EE-B3FF-B5A586E66467}" name="PARAMETERS" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{440FD190-9EC4-4D3D-A87E-66783F143F23}" name="ELAPSED TIME" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{4FF0456A-37BA-4470-B779-0CE6C21F6504}" name="RESULTS" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{28BC94F7-F562-4A52-A433-A77216BAF33C}" name="DATE" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2F3C2F88-E388-48C8-B6EB-07F35CF45C6F}" name="NAME" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1357C874-AE04-46EE-B3FF-B5A586E66467}" name="PARAMETERS" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{440FD190-9EC4-4D3D-A87E-66783F143F23}" name="ELAPSED TIME" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{4FF0456A-37BA-4470-B779-0CE6C21F6504}" name="RESULTS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,21 +589,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F96B11D-0D91-4548-95EE-A8097D08C4D2}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -689,830 +691,830 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87573DA-B50C-46CC-9F7A-94E51E181878}">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
+        <v>12.6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>9.0359999999999996</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.01</v>
+        <v>12.564</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>9.0719999999999992</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.02</v>
+        <v>12.528</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>9.1080000000000005</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.03</v>
+        <v>12.492000000000001</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>9.1440000000000001</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.04</v>
+        <v>12.456</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>9.18</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.05</v>
+        <v>12.42</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>9.2159999999999993</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.06</v>
+        <v>12.384</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>9.2520000000000007</v>
-      </c>
-      <c r="B9" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>12.348000000000001</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9.2880000000000003</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.08</v>
+        <v>12.311999999999999</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>9.3239999999999998</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0.09</v>
+        <v>12.276</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.91</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>9.36</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.1</v>
+        <v>12.24</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>9.3960000000000008</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.11</v>
+        <v>12.204000000000001</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>9.4320000000000004</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.12</v>
+        <v>12.167999999999999</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>9.4679999999999893</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.13</v>
+        <v>12.132</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.87</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>9.5039999999999907</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.14000000000000001</v>
+        <v>12.096</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.86</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>9.5399999999999903</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0.15</v>
+        <v>12.06</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>9.5759999999999899</v>
-      </c>
-      <c r="B18" s="6">
-        <v>0.16</v>
+        <v>12.023999999999999</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>9.6119999999999894</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0.17</v>
+        <v>11.988</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>9.6479999999999908</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0.18</v>
+        <v>11.952</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>9.6839999999999904</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.19</v>
+        <v>11.916</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>9.71999999999999</v>
-      </c>
-      <c r="B22" s="6">
-        <v>0.2</v>
+        <v>11.88</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>9.7559999999999896</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0.21</v>
+        <v>11.843999999999999</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>9.7919999999999892</v>
-      </c>
-      <c r="B24" s="6">
-        <v>0.22</v>
+        <v>11.808</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.78</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>9.8279999999999905</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0.23</v>
+        <v>11.772</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.77</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>9.8639999999999901</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.24</v>
+        <v>11.736000000000001</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>9.8999999999999897</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0.25</v>
+        <v>11.7</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>9.9359999999999893</v>
-      </c>
-      <c r="B28" s="6">
-        <v>0.26</v>
+        <v>11.664</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.74</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>9.9719999999999906</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0.27</v>
+        <v>11.628</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.73</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>10.007999999999999</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0.28000000000000003</v>
+        <v>11.592000000000001</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0.72</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>10.044</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.28999999999999998</v>
+        <v>11.555999999999999</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0.71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>10.08</v>
-      </c>
-      <c r="B32" s="6">
-        <v>0.3</v>
+        <v>11.52</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0.7</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>10.116</v>
-      </c>
-      <c r="B33" s="6">
-        <v>0.31</v>
+        <v>11.484</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0.69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>10.151999999999999</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.32</v>
+        <v>11.448</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0.68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>10.188000000000001</v>
-      </c>
-      <c r="B35" s="6">
-        <v>0.33</v>
+        <v>11.412000000000001</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>10.224</v>
-      </c>
-      <c r="B36" s="6">
-        <v>0.34</v>
+        <v>11.375999999999999</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>10.26</v>
-      </c>
-      <c r="B37" s="6">
-        <v>0.35</v>
+        <v>11.34</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0.65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>10.295999999999999</v>
-      </c>
-      <c r="B38" s="6">
-        <v>0.36</v>
+        <v>11.304</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0.64</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>10.332000000000001</v>
-      </c>
-      <c r="B39" s="6">
-        <v>0.37</v>
+        <v>11.268000000000001</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0.63</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>10.368</v>
-      </c>
-      <c r="B40" s="6">
-        <v>0.38</v>
+        <v>11.231999999999999</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0.62</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>10.404</v>
-      </c>
-      <c r="B41" s="6">
-        <v>0.39</v>
+        <v>11.196</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>10.44</v>
-      </c>
-      <c r="B42" s="6">
-        <v>0.4</v>
+        <v>11.16</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>10.476000000000001</v>
-      </c>
-      <c r="B43" s="6">
-        <v>0.41</v>
+        <v>11.124000000000001</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0.59</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10.512</v>
-      </c>
-      <c r="B44" s="6">
-        <v>0.42</v>
+        <v>11.087999999999999</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>10.548</v>
-      </c>
-      <c r="B45" s="6">
-        <v>0.43</v>
+        <v>11.052</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>10.584</v>
-      </c>
-      <c r="B46" s="6">
-        <v>0.44</v>
+        <v>11.016</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10.62</v>
-      </c>
-      <c r="B47" s="6">
-        <v>0.45</v>
+        <v>10.98</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>10.656000000000001</v>
-      </c>
-      <c r="B48" s="6">
-        <v>0.46</v>
+        <v>10.944000000000001</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0.54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>10.692</v>
-      </c>
-      <c r="B49" s="6">
-        <v>0.47</v>
+        <v>10.907999999999999</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0.53</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>10.728</v>
-      </c>
-      <c r="B50" s="6">
-        <v>0.48</v>
+        <v>10.872</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0.52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>10.763999999999999</v>
-      </c>
-      <c r="B51" s="6">
-        <v>0.49</v>
+        <v>10.836</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0.51</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>10.8</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>10.836</v>
-      </c>
-      <c r="B53" s="6">
-        <v>0.51</v>
+        <v>10.763999999999999</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0.49</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>10.872</v>
-      </c>
-      <c r="B54" s="6">
-        <v>0.52</v>
+        <v>10.728</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0.48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>10.907999999999999</v>
-      </c>
-      <c r="B55" s="6">
-        <v>0.53</v>
+        <v>10.692</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0.47</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>10.944000000000001</v>
-      </c>
-      <c r="B56" s="6">
-        <v>0.54</v>
+        <v>10.656000000000001</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.46</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>10.98</v>
-      </c>
-      <c r="B57" s="6">
-        <v>0.55000000000000004</v>
+        <v>10.62</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0.45</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>11.016</v>
-      </c>
-      <c r="B58" s="6">
-        <v>0.56000000000000005</v>
+        <v>10.584</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.44</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>11.052</v>
-      </c>
-      <c r="B59" s="6">
-        <v>0.56999999999999995</v>
+        <v>10.548</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0.43</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>11.087999999999999</v>
-      </c>
-      <c r="B60" s="6">
-        <v>0.57999999999999996</v>
+        <v>10.512</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0.42</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>11.124000000000001</v>
-      </c>
-      <c r="B61" s="6">
-        <v>0.59</v>
+        <v>10.476000000000001</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.41</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>11.16</v>
-      </c>
-      <c r="B62" s="6">
-        <v>0.6</v>
+        <v>10.44</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>11.196</v>
-      </c>
-      <c r="B63" s="6">
-        <v>0.61</v>
+        <v>10.404</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0.39</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>11.231999999999999</v>
-      </c>
-      <c r="B64" s="6">
-        <v>0.62</v>
+        <v>10.368</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0.38</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>11.268000000000001</v>
-      </c>
-      <c r="B65" s="6">
-        <v>0.63</v>
+        <v>10.332000000000001</v>
+      </c>
+      <c r="B65" s="5">
+        <v>0.37</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>11.304</v>
-      </c>
-      <c r="B66" s="6">
-        <v>0.64</v>
+        <v>10.295999999999999</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0.36</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>11.34</v>
-      </c>
-      <c r="B67" s="6">
-        <v>0.65</v>
+        <v>10.26</v>
+      </c>
+      <c r="B67" s="5">
+        <v>0.35</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>11.375999999999999</v>
-      </c>
-      <c r="B68" s="6">
-        <v>0.66</v>
+        <v>10.224</v>
+      </c>
+      <c r="B68" s="5">
+        <v>0.34</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>11.412000000000001</v>
-      </c>
-      <c r="B69" s="6">
-        <v>0.67</v>
+        <v>10.188000000000001</v>
+      </c>
+      <c r="B69" s="5">
+        <v>0.33</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>11.448</v>
-      </c>
-      <c r="B70" s="6">
-        <v>0.68</v>
+        <v>10.151999999999999</v>
+      </c>
+      <c r="B70" s="5">
+        <v>0.32</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>11.484</v>
-      </c>
-      <c r="B71" s="6">
-        <v>0.69</v>
+        <v>10.116</v>
+      </c>
+      <c r="B71" s="5">
+        <v>0.31</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>11.52</v>
-      </c>
-      <c r="B72" s="6">
-        <v>0.7</v>
+        <v>10.08</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0.3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>11.555999999999999</v>
-      </c>
-      <c r="B73" s="6">
-        <v>0.71</v>
+        <v>10.044</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>11.592000000000001</v>
-      </c>
-      <c r="B74" s="6">
-        <v>0.72</v>
+        <v>10.007999999999999</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>11.628</v>
-      </c>
-      <c r="B75" s="6">
-        <v>0.73</v>
+        <v>9.9719999999999906</v>
+      </c>
+      <c r="B75" s="5">
+        <v>0.27</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>11.664</v>
-      </c>
-      <c r="B76" s="6">
-        <v>0.74</v>
+        <v>9.9359999999999893</v>
+      </c>
+      <c r="B76" s="5">
+        <v>0.26</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>11.7</v>
-      </c>
-      <c r="B77" s="6">
-        <v>0.75</v>
+        <v>9.8999999999999897</v>
+      </c>
+      <c r="B77" s="5">
+        <v>0.25</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>11.736000000000001</v>
-      </c>
-      <c r="B78" s="6">
-        <v>0.76</v>
+        <v>9.8639999999999901</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0.24</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>11.772</v>
-      </c>
-      <c r="B79" s="6">
-        <v>0.77</v>
+        <v>9.8279999999999905</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0.23</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>11.808</v>
-      </c>
-      <c r="B80" s="6">
-        <v>0.78</v>
+        <v>9.7919999999999892</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0.22</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>11.843999999999999</v>
-      </c>
-      <c r="B81" s="6">
-        <v>0.79</v>
+        <v>9.7559999999999896</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0.21</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>11.88</v>
-      </c>
-      <c r="B82" s="6">
-        <v>0.8</v>
+        <v>9.71999999999999</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0.2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>11.916</v>
-      </c>
-      <c r="B83" s="6">
-        <v>0.81</v>
+        <v>9.6839999999999904</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0.19</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>11.952</v>
-      </c>
-      <c r="B84" s="6">
-        <v>0.82</v>
+        <v>9.6479999999999908</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0.18</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>11.988</v>
-      </c>
-      <c r="B85" s="6">
-        <v>0.83</v>
+        <v>9.6119999999999894</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0.17</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>12.023999999999999</v>
-      </c>
-      <c r="B86" s="6">
-        <v>0.84</v>
+        <v>9.5759999999999899</v>
+      </c>
+      <c r="B86" s="5">
+        <v>0.16</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>12.06</v>
-      </c>
-      <c r="B87" s="6">
-        <v>0.85</v>
+        <v>9.5399999999999903</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0.15</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>12.096</v>
-      </c>
-      <c r="B88" s="6">
-        <v>0.86</v>
+        <v>9.5039999999999907</v>
+      </c>
+      <c r="B88" s="5">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>12.132</v>
-      </c>
-      <c r="B89" s="6">
-        <v>0.87</v>
+        <v>9.4679999999999893</v>
+      </c>
+      <c r="B89" s="5">
+        <v>0.13</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>12.167999999999999</v>
-      </c>
-      <c r="B90" s="6">
-        <v>0.88</v>
+        <v>9.4320000000000004</v>
+      </c>
+      <c r="B90" s="5">
+        <v>0.12</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>12.204000000000001</v>
-      </c>
-      <c r="B91" s="6">
-        <v>0.89</v>
+        <v>9.3960000000000008</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0.11</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>12.24</v>
-      </c>
-      <c r="B92" s="6">
-        <v>0.9</v>
+        <v>9.36</v>
+      </c>
+      <c r="B92" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>12.276</v>
-      </c>
-      <c r="B93" s="6">
-        <v>0.91</v>
+        <v>9.3239999999999998</v>
+      </c>
+      <c r="B93" s="5">
+        <v>0.09</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>12.311999999999999</v>
-      </c>
-      <c r="B94" s="6">
-        <v>0.92</v>
+        <v>9.2880000000000003</v>
+      </c>
+      <c r="B94" s="5">
+        <v>0.08</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>12.348000000000001</v>
-      </c>
-      <c r="B95" s="6">
-        <v>0.93</v>
+        <v>9.2520000000000007</v>
+      </c>
+      <c r="B95" s="5">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>12.384</v>
-      </c>
-      <c r="B96" s="6">
-        <v>0.94</v>
+        <v>9.2159999999999993</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.06</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>12.42</v>
-      </c>
-      <c r="B97" s="6">
-        <v>0.95</v>
+        <v>9.18</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>12.456</v>
-      </c>
-      <c r="B98" s="6">
-        <v>0.96</v>
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0.04</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>12.492000000000001</v>
-      </c>
-      <c r="B99" s="6">
-        <v>0.97</v>
+        <v>9.1080000000000005</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0.03</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>12.528</v>
-      </c>
-      <c r="B100" s="6">
-        <v>0.98</v>
+        <v>9.0719999999999992</v>
+      </c>
+      <c r="B100" s="5">
+        <v>0.02</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>12.564</v>
-      </c>
-      <c r="B101" s="6">
-        <v>0.99</v>
+        <v>9.0359999999999996</v>
+      </c>
+      <c r="B101" s="5">
+        <v>0.01</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>12.6</v>
-      </c>
-      <c r="B102" s="6">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B102" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1533,21 +1535,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
@@ -1567,7 +1569,7 @@
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1578,28 +1580,28 @@
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
     </row>
   </sheetData>

</xml_diff>